<commit_message>
add 柱形图/ fix bug
</commit_message>
<xml_diff>
--- a/example/text.xlsx
+++ b/example/text.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
     <t>title</t>
   </si>
@@ -22,28 +22,34 @@
     <t>label</t>
   </si>
   <si>
-    <t>life</t>
-  </si>
-  <si>
-    <t>生活学会了坚强</t>
-  </si>
-  <si>
-    <t>饭前刷牙</t>
-  </si>
-  <si>
-    <t>medicine</t>
-  </si>
-  <si>
-    <t>测试生活</t>
-  </si>
-  <si>
-    <t>dadas</t>
-  </si>
-  <si>
-    <t>dasdasd</t>
-  </si>
-  <si>
-    <t>activity img</t>
+    <t>test_10</t>
+  </si>
+  <si>
+    <t>test_11</t>
+  </si>
+  <si>
+    <t>test_12</t>
+  </si>
+  <si>
+    <t>test_13</t>
+  </si>
+  <si>
+    <t>test_14</t>
+  </si>
+  <si>
+    <t>test_15</t>
+  </si>
+  <si>
+    <t>test_16</t>
+  </si>
+  <si>
+    <t>test_17</t>
+  </si>
+  <si>
+    <t>test_18</t>
+  </si>
+  <si>
+    <t>test_19</t>
   </si>
 </sst>
 </file>
@@ -399,112 +405,80 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
+      <c r="B2" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
+      <c r="B3" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>5</v>
+      <c r="B4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>2</v>
+        <v>9</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>2</v>
+        <v>10</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" t="s">
-        <v>2</v>
+        <v>11</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>